<commit_message>
implemented markdown inline formatting
</commit_message>
<xml_diff>
--- a/dev/Book1.xlsx
+++ b/dev/Book1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/denisdreano/knitxl/dev/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6D5C0B0B-0F7F-1349-8A89-3C8EC8936EDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29499C98-30C1-EC42-BDF7-5EE6A6E41CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11580" yWindow="5400" windowWidth="28040" windowHeight="17440" xr2:uid="{CB6B7F8E-1462-C148-8C73-663967A7AFD9}"/>
+    <workbookView xWindow="1960" yWindow="4980" windowWidth="28040" windowHeight="17440" xr2:uid="{CB6B7F8E-1462-C148-8C73-663967A7AFD9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,20 +38,37 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>title</t>
+    <r>
+      <t xml:space="preserve">lorem </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>ipsum</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="2">
@@ -393,7 +410,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>